<commit_message>
close #98: Improve spell check and add extra words
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth/descricao.xlsx
+++ b/input_data/data_ground_truth/descricao.xlsx
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Variações climáticas relacionadas à seca, com base em um intervalo climático normal de 30 anos.</t>
   </si>
   <si>
-    <t xml:space="preserve">O sistema socioecológico é um dos componentes do sistema terrestre expostos às ameaças climáticas como a seca. Por convenção, o termo ameaça climática no AdaptaBrasil MCTI será utilizado para denotar fatores externos (especificamente climáticos) que interagem com o sistema socioecológico analisado e que possuem capacidade de impactar de forma significativa o sistema, seja de forma lenta ou repentina. O Índice de Ameaça Climática para a seca é resultante da composição do número de dias consecutivos secos e do Índice de Precipitação-Evapotranspiração Padronizado (do acrônimo em inglês Standardized Precipitation-Evapotranspiration Index – SPEI). Devido à utilização de uma faixa de valores do SPEI que expressam padrões de seca (valores inferiores a -0,5), os valores superiores a -0,5 foram desconsiderados e receberam NA (do inglês Not Available ou Não Disponível em tradução livre), visto que os mesmos caracterizam normalidade ou excessos de chuvas quando ponderada a precipitação. No resultado final do índice, os valores NA foram substituídos por 0 (zero), visto que isso representa a ausência de padrões de seca.&lt;br&gt;&lt;br&gt;Fontes:&lt;br&gt;GALLOPÍN, G. C.. Box 1: A systemic synthesis of the relations between vulnerability, hazard, exposure and impact, aimed at policy identification. In: Economic Commission for Latin American and the Caribbean (ECLAC). Handbook for Estimating the Socio-Economic and Environmental Effects of Disasters. Mexico, D.F.: ECLAC, LC/MEX/G.S., p. 2-5, 2003.&lt;br&gt;INTERGOVERNMENTAL PANEL ON CLIMATE CHANGE - IPCC. Climate Change 2014: Synthesis Report. Working Groups I, II and III to the Fifth Assessment Report of the Intergovernmental Panel on Climate Change [Core Writing Team, R.K. Pachauri and L.A. Meyer (eds.)]. IPCC, Geneva, Switzerland, 151 pp.</t>
+    <t xml:space="preserve">O sistema socioecológico é um dos componentes do sistema terrestre expostos às ameaças climáticas como a seca. Por convenção, o termo ameaça climática no AdaptaBrasil será utilizado para denotar fatores externos (especificamente climáticos) que interagem com o sistema socioecológico analisado e que possuem capacidade de impactar de forma significativa o sistema, seja de forma lenta ou repentina. O Índice de Ameaça Climática para a seca é resultante da composição do número de dias consecutivos secos e do Índice de Precipitação-Evapotranspiração Padronizado (do acrônimo em inglês Standardized Precipitation-Evapotranspiration Index). Devido à utilização de uma faixa de valores do AdaptaBrasil que expressam padrões de seca (valores inferiores a -0,5), os valores superiores a -0,5 foram desconsiderados e receberam NA (do inglês Not Available ou Não Disponível em tradução livre), visto que os mesmos caracterizam normalidade ou excessos de chuvas quando ponderada a precipitação. No resultado final do índice, os valores NA foram substituídos por 0 (zero), visto que isso representa a ausência de padrões de seca.&lt;br&gt;&lt;br&gt;Fontes:&lt;br&gt;GALLOPÍN, G. C.. Box 1: A systemic synthesis of the relations between vulnerability, hazard, exposure and impact, aimed at policy identification. In: Economic Commission for Latin American and the Caribbean (ECLAC). Handbook for Estimating the Socio-Economic and Environmental Effects of Disasters. Mexico, D.F.: ECLAC, LC/MEX/G.S., p. 2-5, 2003.&lt;br&gt;INTERGOVERNMENTAL PANEL ON CLIMATE CHANGE - IPCC. Climate Change 2014: Synthesis Report. Working Groups I, II and III to the Fifth Assessment Report of the Intergovernmental Panel on Climate Change [Core Writing Team, R.K. Pachauri and L.A. Meyer (eds.)]. IPCC, Geneva, Switzerland, 151 pp.</t>
   </si>
   <si>
     <t xml:space="preserve">4.3,6.3</t>
@@ -404,21 +404,21 @@
   </sheetPr>
   <dimension ref="A1:Y866"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="27.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="126.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="102.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="126.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="102.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="24.57"/>

</xml_diff>